<commit_message>
visualization and tfe figures
</commit_message>
<xml_diff>
--- a/results_class.xlsx
+++ b/results_class.xlsx
@@ -4,42 +4,26 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="cvt_32" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="47_byol" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
-      <charset val="1"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b val="1"/>
@@ -68,32 +52,19 @@
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -450,31 +421,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="0" outlineLevelRow="0"/>
-  <sheetData/>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M68"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +494,11 @@
           <t>t_search</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>t_transfer</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -551,40 +507,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9410826166478578</v>
+        <v>0.9511226991477605</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9904268980814881</v>
+        <v>0.989570767015605</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9908938786628789</v>
+        <v>0.9767677160758065</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9961863252519749</v>
+        <v>0.994045997587267</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9908938786628789</v>
+        <v>0.9767677160758065</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9961863252519749</v>
+        <v>0.994045997587267</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9575436821418842</v>
+        <v>0.9631474491185742</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9914776043896175</v>
+        <v>0.9803479005331361</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9914776043896175</v>
+        <v>0.9803479005331361</v>
       </c>
       <c r="K2" t="n">
-        <v>833.6186628341675</v>
+        <v>212.8395810127258</v>
       </c>
       <c r="L2" t="n">
-        <v>442.7138707637787</v>
+        <v>64.68518471717834</v>
       </c>
       <c r="M2" t="n">
-        <v>293.2796766757965</v>
+        <v>138.7499406337738</v>
+      </c>
+      <c r="N2" t="n">
+        <v>7.284701108932495</v>
       </c>
     </row>
     <row r="3">
@@ -594,40 +553,43 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4598313359964492</v>
+        <v>0.3266755437194852</v>
       </c>
       <c r="C3" t="n">
-        <v>0.711051930758988</v>
+        <v>0.5876608965823347</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9995561473590768</v>
+        <v>0.8317798490901021</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0.9196626719928983</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9995561473590768</v>
+        <v>0.8317798490901021</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>0.9196626719928983</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4536173990235242</v>
+        <v>0.3559698180204172</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0.8477585441633377</v>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>0.8477585441633377</v>
       </c>
       <c r="K3" t="n">
-        <v>70.98800420761108</v>
+        <v>18.77217221260071</v>
       </c>
       <c r="L3" t="n">
-        <v>37.15366697311401</v>
+        <v>5.61884069442749</v>
       </c>
       <c r="M3" t="n">
-        <v>25.53284597396851</v>
+        <v>12.33179235458374</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.6405248641967773</v>
       </c>
     </row>
     <row r="4">
@@ -637,40 +599,43 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.6776859504132231</v>
+        <v>0.628099173553719</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9752066115702479</v>
+        <v>0.9421487603305785</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9917355371900827</v>
+        <v>0.8429752066115702</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0.9586776859504132</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0.8429752066115702</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0.9669421487603306</v>
       </c>
       <c r="H4" t="n">
+        <v>0.6446280991735537</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.8016528925619835</v>
       </c>
-      <c r="I4" t="n">
-        <v>0.9917355371900827</v>
-      </c>
       <c r="J4" t="n">
-        <v>0.9917355371900827</v>
+        <v>0.8016528925619835</v>
       </c>
       <c r="K4" t="n">
-        <v>3.387266874313354</v>
+        <v>1.018982172012329</v>
       </c>
       <c r="L4" t="n">
-        <v>1.953148603439331</v>
+        <v>0.3108024597167969</v>
       </c>
       <c r="M4" t="n">
-        <v>1.389384269714355</v>
+        <v>0.6638228893280029</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.03403687477111816</v>
       </c>
     </row>
     <row r="5">
@@ -680,40 +645,43 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5961538461538461</v>
+        <v>0.2884615384615384</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8846153846153846</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="D5" t="n">
+        <v>0.8653846153846154</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.9807692307692307</v>
       </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
       <c r="F5" t="n">
+        <v>0.8653846153846154</v>
+      </c>
+      <c r="G5" t="n">
         <v>0.9807692307692307</v>
       </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
       <c r="H5" t="n">
-        <v>0.4423076923076923</v>
+        <v>0.1538461538461539</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>0.8653846153846154</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>0.8653846153846154</v>
       </c>
       <c r="K5" t="n">
-        <v>1.441197156906128</v>
+        <v>0.4461154937744141</v>
       </c>
       <c r="L5" t="n">
-        <v>0.8291110992431641</v>
+        <v>0.1343374252319336</v>
       </c>
       <c r="M5" t="n">
-        <v>0.5885953903198242</v>
+        <v>0.2920017242431641</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.01500821113586426</v>
       </c>
     </row>
     <row r="6">
@@ -723,40 +691,43 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9412673879443586</v>
+        <v>0.9036579082946935</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9922720247295209</v>
+        <v>0.9752704791344667</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9933024214322514</v>
+        <v>0.9453889747552808</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9969088098918083</v>
+        <v>0.979392065945389</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9933024214322514</v>
+        <v>0.9453889747552808</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9969088098918083</v>
+        <v>0.979392065945389</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9608449252962391</v>
+        <v>0.9103554868624421</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9948480164863472</v>
+        <v>0.9422977846470891</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9948480164863472</v>
+        <v>0.9422977846470891</v>
       </c>
       <c r="K6" t="n">
-        <v>55.92451214790344</v>
+        <v>16.33702564239502</v>
       </c>
       <c r="L6" t="n">
-        <v>31.6705756187439</v>
+        <v>4.96305251121521</v>
       </c>
       <c r="M6" t="n">
-        <v>22.09388995170593</v>
+        <v>10.6593132019043</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5518434047698975</v>
       </c>
     </row>
     <row r="7">
@@ -766,40 +737,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.7238658777120316</v>
+        <v>0.6173570019723866</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9211045364891519</v>
+        <v>0.8619329388560157</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.9881656804733728</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0.9980276134122288</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>0.9881656804733728</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>0.9980276134122288</v>
       </c>
       <c r="H7" t="n">
-        <v>0.727810650887574</v>
+        <v>0.5838264299802761</v>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0.9881656804733728</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>0.9881656804733728</v>
       </c>
       <c r="K7" t="n">
-        <v>14.23236513137817</v>
+        <v>4.270281791687012</v>
       </c>
       <c r="L7" t="n">
-        <v>8.168169975280762</v>
+        <v>1.295429944992065</v>
       </c>
       <c r="M7" t="n">
-        <v>5.772198677062988</v>
+        <v>2.789364099502563</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.142888069152832</v>
       </c>
     </row>
     <row r="8">
@@ -809,40 +783,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5952380952380952</v>
+        <v>0.5158730158730159</v>
       </c>
       <c r="C8" t="n">
-        <v>0.876984126984127</v>
+        <v>0.746031746031746</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0.7023809523809523</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>0.8611111111111112</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0.7023809523809523</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>0.8611111111111112</v>
       </c>
       <c r="H8" t="n">
-        <v>0.5515873015873016</v>
+        <v>0.3373015873015873</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0.5753968253968254</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>0.5753968253968254</v>
       </c>
       <c r="K8" t="n">
-        <v>9.132504940032959</v>
+        <v>2.122107267379761</v>
       </c>
       <c r="L8" t="n">
-        <v>4.683303594589233</v>
+        <v>0.6312263011932373</v>
       </c>
       <c r="M8" t="n">
-        <v>2.899371147155762</v>
+        <v>1.397303819656372</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.07161235809326172</v>
       </c>
     </row>
     <row r="9">
@@ -852,40 +829,43 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.3083333333333333</v>
+        <v>0.225</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5583333333333333</v>
+        <v>0.4083333333333333</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0.7166666666666667</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0.8416666666666667</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>0.7166666666666667</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>0.8416666666666667</v>
       </c>
       <c r="H9" t="n">
-        <v>0.175</v>
+        <v>0.1416666666666667</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="K9" t="n">
-        <v>4.243816137313843</v>
+        <v>1.020384311676025</v>
       </c>
       <c r="L9" t="n">
-        <v>2.159253597259521</v>
+        <v>0.3021490573883057</v>
       </c>
       <c r="M9" t="n">
-        <v>1.367741823196411</v>
+        <v>0.674553394317627</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.0334620475769043</v>
       </c>
     </row>
     <row r="10">
@@ -895,40 +875,43 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.35</v>
+        <v>0.3125</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7625</v>
+        <v>0.5</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9708333333333333</v>
+        <v>0.4833333333333333</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9875</v>
+        <v>0.7041666666666667</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9708333333333333</v>
+        <v>0.4833333333333333</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9875</v>
+        <v>0.7041666666666667</v>
       </c>
       <c r="H10" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.2125</v>
       </c>
       <c r="I10" t="n">
-        <v>0.9666666666666667</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="J10" t="n">
-        <v>0.9666666666666667</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="K10" t="n">
-        <v>8.525515556335449</v>
+        <v>2.013687610626221</v>
       </c>
       <c r="L10" t="n">
-        <v>4.314181566238403</v>
+        <v>0.6041021347045898</v>
       </c>
       <c r="M10" t="n">
-        <v>2.736140489578247</v>
+        <v>1.321465730667114</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.06723499298095703</v>
       </c>
     </row>
     <row r="11">
@@ -938,40 +921,43 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.3981481481481481</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.7129629629629629</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.7129629629629629</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.09259259259259259</v>
+      </c>
+      <c r="I11" t="n">
         <v>0.2592592592592592</v>
       </c>
-      <c r="C11" t="n">
-        <v>0.6944444444444444</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.9907407407407407</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.9907407407407407</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.1296296296296296</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.9907407407407407</v>
-      </c>
       <c r="J11" t="n">
-        <v>0.9907407407407407</v>
+        <v>0.2592592592592592</v>
       </c>
       <c r="K11" t="n">
-        <v>3.901757955551147</v>
+        <v>0.9129822254180908</v>
       </c>
       <c r="L11" t="n">
-        <v>1.964615821838379</v>
+        <v>0.2724268436431885</v>
       </c>
       <c r="M11" t="n">
-        <v>1.24616265296936</v>
+        <v>0.6008379459381104</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.03023672103881836</v>
       </c>
     </row>
     <row r="12">
@@ -981,40 +967,43 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.5537098560354374</v>
+        <v>0.3444075304540421</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9712070874861573</v>
+        <v>0.7187153931339978</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9928017718715393</v>
+        <v>0.6611295681063123</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9977851605758582</v>
+        <v>0.8588039867109635</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9950166112956811</v>
+        <v>0.7823920265780731</v>
       </c>
       <c r="G12" t="n">
-        <v>0.9994462901439646</v>
+        <v>0.9335548172757475</v>
       </c>
       <c r="H12" t="n">
-        <v>0.6018826135105205</v>
+        <v>0.3156146179401993</v>
       </c>
       <c r="I12" t="n">
-        <v>0.9944629014396457</v>
+        <v>0.6810631229235881</v>
       </c>
       <c r="J12" t="n">
-        <v>0.9977851605758582</v>
+        <v>0.8167220376522702</v>
       </c>
       <c r="K12" t="n">
-        <v>54.06699633598328</v>
+        <v>15.01774549484253</v>
       </c>
       <c r="L12" t="n">
-        <v>30.25708270072937</v>
+        <v>4.604691028594971</v>
       </c>
       <c r="M12" t="n">
-        <v>20.74234843254089</v>
+        <v>9.833874702453613</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.4316787719726562</v>
       </c>
     </row>
     <row r="13">
@@ -1024,40 +1013,43 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4855233853006681</v>
+        <v>0.3392724573125464</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8901262063845583</v>
+        <v>0.7048997772828508</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9283593170007424</v>
+        <v>0.566815144766147</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9402375649591685</v>
+        <v>0.7858203414996288</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9342984409799554</v>
+        <v>0.6655530809205642</v>
       </c>
       <c r="G13" t="n">
-        <v>0.947290274684484</v>
+        <v>0.8685968819599109</v>
       </c>
       <c r="H13" t="n">
-        <v>0.4792130660727543</v>
+        <v>0.325909428359317</v>
       </c>
       <c r="I13" t="n">
-        <v>0.9328136599851522</v>
+        <v>0.5734966592427617</v>
       </c>
       <c r="J13" t="n">
-        <v>0.9420935412026726</v>
+        <v>0.6904231625835189</v>
       </c>
       <c r="K13" t="n">
-        <v>80.60603260993958</v>
+        <v>22.38696885108948</v>
       </c>
       <c r="L13" t="n">
-        <v>45.02424120903015</v>
+        <v>6.784338474273682</v>
       </c>
       <c r="M13" t="n">
-        <v>30.88445830345154</v>
+        <v>14.67325258255005</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.7039890289306641</v>
       </c>
     </row>
     <row r="14">
@@ -1067,40 +1059,43 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3714285714285714</v>
+        <v>0.6761904761904762</v>
       </c>
       <c r="C14" t="n">
-        <v>0.780952380952381</v>
+        <v>0.8952380952380953</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0.8761904761904762</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>0.9904761904761905</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>0.8761904761904762</v>
       </c>
       <c r="G14" t="n">
-        <v>1</v>
+        <v>0.9904761904761905</v>
       </c>
       <c r="H14" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.6476190476190476</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0.9047619047619048</v>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>0.9047619047619048</v>
       </c>
       <c r="K14" t="n">
-        <v>3.139862298965454</v>
+        <v>0.8856766223907471</v>
       </c>
       <c r="L14" t="n">
-        <v>1.816736459732056</v>
+        <v>0.2725117206573486</v>
       </c>
       <c r="M14" t="n">
-        <v>1.202571630477905</v>
+        <v>0.5814671516418457</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.02241635322570801</v>
       </c>
     </row>
     <row r="15">
@@ -1110,40 +1105,43 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.36</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9966666666666667</v>
+        <v>0.6133333333333333</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0.5733333333333334</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0.72</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>0.5733333333333334</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>0.72</v>
       </c>
       <c r="H15" t="n">
-        <v>0.9633333333333334</v>
+        <v>0.39</v>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0.6533333333333333</v>
       </c>
       <c r="J15" t="n">
-        <v>1</v>
+        <v>0.6533333333333333</v>
       </c>
       <c r="K15" t="n">
-        <v>8.719830751419067</v>
+        <v>2.532343864440918</v>
       </c>
       <c r="L15" t="n">
-        <v>4.93941593170166</v>
+        <v>0.7754738330841064</v>
       </c>
       <c r="M15" t="n">
-        <v>3.428502321243286</v>
+        <v>1.655122041702271</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.07612133026123047</v>
       </c>
     </row>
     <row r="16">
@@ -1153,40 +1151,43 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.09807640205906258</v>
+        <v>0.0999729070712544</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3695475480899485</v>
+        <v>0.2801408832294771</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1303169872663235</v>
+        <v>0.1110810078569493</v>
       </c>
       <c r="E16" t="n">
-        <v>0.4196694662693037</v>
+        <v>0.301544296938499</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1305879165537795</v>
+        <v>0.2351666215117854</v>
       </c>
       <c r="G16" t="n">
-        <v>0.4199403955567597</v>
+        <v>0.4554321322134923</v>
       </c>
       <c r="H16" t="n">
-        <v>0.04632890815497155</v>
+        <v>0.05256028176645895</v>
       </c>
       <c r="I16" t="n">
-        <v>0.07938228122460038</v>
+        <v>0.07233811975074506</v>
       </c>
       <c r="J16" t="n">
-        <v>0.07965321051205636</v>
+        <v>0.2145759956651314</v>
       </c>
       <c r="K16" t="n">
-        <v>110.869900226593</v>
+        <v>30.809809923172</v>
       </c>
       <c r="L16" t="n">
-        <v>61.52869057655334</v>
+        <v>9.229090213775635</v>
       </c>
       <c r="M16" t="n">
-        <v>42.24990606307983</v>
+        <v>20.27598524093628</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1.001186370849609</v>
       </c>
     </row>
     <row r="17">
@@ -1196,40 +1197,43 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.03604651162790698</v>
+        <v>0.005813953488372093</v>
       </c>
       <c r="C17" t="n">
-        <v>0.113953488372093</v>
+        <v>0.03255813953488372</v>
       </c>
       <c r="D17" t="n">
-        <v>0.09302325581395349</v>
+        <v>0.05813953488372093</v>
       </c>
       <c r="E17" t="n">
-        <v>0.3313953488372093</v>
+        <v>0.1906976744186047</v>
       </c>
       <c r="F17" t="n">
-        <v>0.09302325581395349</v>
+        <v>0.1406976744186046</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3313953488372093</v>
+        <v>0.2988372093023256</v>
       </c>
       <c r="H17" t="n">
-        <v>0.01046511627906977</v>
+        <v>0.002325581395348837</v>
       </c>
       <c r="I17" t="n">
-        <v>0.06046511627906977</v>
+        <v>0.03837209302325582</v>
       </c>
       <c r="J17" t="n">
-        <v>0.06046511627906977</v>
+        <v>0.1406976744186046</v>
       </c>
       <c r="K17" t="n">
-        <v>25.43958449363708</v>
+        <v>7.211183547973633</v>
       </c>
       <c r="L17" t="n">
-        <v>14.14086174964905</v>
+        <v>2.181328058242798</v>
       </c>
       <c r="M17" t="n">
-        <v>9.877539396286011</v>
+        <v>4.733300924301147</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.2246263027191162</v>
       </c>
     </row>
     <row r="18">
@@ -1239,40 +1243,43 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.8401562020095652</v>
+        <v>0.8656925979553333</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9802992409284367</v>
+        <v>0.9860910008336624</v>
       </c>
       <c r="D18" t="n">
-        <v>0.99482251766048</v>
+        <v>0.9996051072791892</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9986836909306305</v>
+        <v>0.999956123031021</v>
       </c>
       <c r="F18" t="n">
-        <v>0.994866394629459</v>
+        <v>0.9996051072791892</v>
       </c>
       <c r="G18" t="n">
-        <v>0.9987714448685885</v>
+        <v>0.999956123031021</v>
       </c>
       <c r="H18" t="n">
-        <v>0.8812250449738932</v>
+        <v>0.9089114123996315</v>
       </c>
       <c r="I18" t="n">
-        <v>0.9955684261331227</v>
+        <v>0.9996928612171471</v>
       </c>
       <c r="J18" t="n">
-        <v>0.9957000570400597</v>
+        <v>0.9996928612171471</v>
       </c>
       <c r="K18" t="n">
-        <v>640.9322712421417</v>
+        <v>191.3361597061157</v>
       </c>
       <c r="L18" t="n">
-        <v>372.4428834915161</v>
+        <v>58.19069576263428</v>
       </c>
       <c r="M18" t="n">
-        <v>260.456652879715</v>
+        <v>124.8124074935913</v>
+      </c>
+      <c r="N18" t="n">
+        <v>6.445091009140015</v>
       </c>
     </row>
     <row r="19">
@@ -1282,40 +1289,43 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.614435261707989</v>
+        <v>0.548870523415978</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9358677685950413</v>
+        <v>0.8643526170798899</v>
       </c>
       <c r="D19" t="n">
-        <v>0.9988980716253444</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9988980716253444</v>
+        <v>1</v>
       </c>
       <c r="G19" t="n">
         <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>0.6802203856749311</v>
+        <v>0.5866666666666667</v>
       </c>
       <c r="I19" t="n">
-        <v>0.9995592286501377</v>
+        <v>1</v>
       </c>
       <c r="J19" t="n">
-        <v>0.9995592286501377</v>
+        <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>252.021785736084</v>
+        <v>77.64649081230164</v>
       </c>
       <c r="L19" t="n">
-        <v>146.0455543994904</v>
+        <v>23.17767810821533</v>
       </c>
       <c r="M19" t="n">
-        <v>103.4185876846313</v>
+        <v>51.12304520606995</v>
+      </c>
+      <c r="N19" t="n">
+        <v>2.595865964889526</v>
       </c>
     </row>
     <row r="20">
@@ -1325,40 +1335,43 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.7575757575757576</v>
+        <v>0.5984848484848485</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9772727272727273</v>
+        <v>0.8787878787878788</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0.8939393939393939</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0.9621212121212122</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>0.8939393939393939</v>
       </c>
       <c r="G20" t="n">
-        <v>1</v>
+        <v>0.9621212121212122</v>
       </c>
       <c r="H20" t="n">
-        <v>0.7348484848484849</v>
+        <v>0.553030303030303</v>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0.8939393939393939</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>0.8939393939393939</v>
       </c>
       <c r="K20" t="n">
-        <v>4.197978734970093</v>
+        <v>1.103074789047241</v>
       </c>
       <c r="L20" t="n">
-        <v>2.24696946144104</v>
+        <v>0.3306176662445068</v>
       </c>
       <c r="M20" t="n">
-        <v>1.502384901046753</v>
+        <v>0.724433422088623</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.03710079193115234</v>
       </c>
     </row>
     <row r="21">
@@ -1368,40 +1381,43 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.896551724137931</v>
+        <v>0.6781609195402298</v>
       </c>
       <c r="C21" t="n">
-        <v>0.9942528735632183</v>
+        <v>0.8908045977011494</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0.8620689655172413</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>0.9540229885057471</v>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>0.867816091954023</v>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>0.9597701149425287</v>
       </c>
       <c r="H21" t="n">
-        <v>0.896551724137931</v>
+        <v>0.6264367816091954</v>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>0.8908045977011494</v>
       </c>
       <c r="J21" t="n">
-        <v>1</v>
+        <v>0.8908045977011494</v>
       </c>
       <c r="K21" t="n">
-        <v>5.486231327056885</v>
+        <v>1.492734909057617</v>
       </c>
       <c r="L21" t="n">
-        <v>2.901411294937134</v>
+        <v>0.4423243999481201</v>
       </c>
       <c r="M21" t="n">
-        <v>1.995861053466797</v>
+        <v>0.9865283966064453</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.04873895645141602</v>
       </c>
     </row>
     <row r="22">
@@ -1411,40 +1427,43 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.82</v>
+        <v>0.5733333333333334</v>
       </c>
       <c r="C22" t="n">
-        <v>0.9733333333333334</v>
+        <v>0.86</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F22" t="n">
-        <v>1</v>
+        <v>0.9266666666666666</v>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="H22" t="n">
-        <v>0.6866666666666666</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0.9066666666666666</v>
       </c>
       <c r="J22" t="n">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="K22" t="n">
-        <v>4.693546295166016</v>
+        <v>1.328896284103394</v>
       </c>
       <c r="L22" t="n">
-        <v>2.483249187469482</v>
+        <v>0.3817131519317627</v>
       </c>
       <c r="M22" t="n">
-        <v>1.699277877807617</v>
+        <v>0.8918852806091309</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.04221963882446289</v>
       </c>
     </row>
     <row r="23">
@@ -1454,40 +1473,43 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.967741935483871</v>
+        <v>0.931899641577061</v>
       </c>
       <c r="C23" t="n">
-        <v>0.992831541218638</v>
+        <v>0.9605734767025089</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0.9390681003584229</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0.96415770609319</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>0.9390681003584229</v>
       </c>
       <c r="G23" t="n">
-        <v>1</v>
+        <v>0.96415770609319</v>
       </c>
       <c r="H23" t="n">
-        <v>0.967741935483871</v>
+        <v>0.9068100358422939</v>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0.9139784946236559</v>
       </c>
       <c r="J23" t="n">
-        <v>1</v>
+        <v>0.9139784946236559</v>
       </c>
       <c r="K23" t="n">
-        <v>8.911733150482178</v>
+        <v>2.361727476119995</v>
       </c>
       <c r="L23" t="n">
-        <v>4.743295907974243</v>
+        <v>0.7097618579864502</v>
       </c>
       <c r="M23" t="n">
-        <v>3.155529260635376</v>
+        <v>1.55059814453125</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.07723546028137207</v>
       </c>
     </row>
     <row r="24">
@@ -1497,40 +1519,43 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.9609375</v>
+        <v>0.90625</v>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>0.953125</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>0.9140625</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>0.953125</v>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>0.9140625</v>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
+        <v>0.953125</v>
       </c>
       <c r="H24" t="n">
-        <v>1</v>
+        <v>0.8828125</v>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0.90625</v>
       </c>
       <c r="J24" t="n">
-        <v>1</v>
+        <v>0.90625</v>
       </c>
       <c r="K24" t="n">
-        <v>4.065872669219971</v>
+        <v>1.126624822616577</v>
       </c>
       <c r="L24" t="n">
-        <v>2.19454026222229</v>
+        <v>0.3282723426818848</v>
       </c>
       <c r="M24" t="n">
-        <v>1.459194421768188</v>
+        <v>0.7521862983703613</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.03450441360473633</v>
       </c>
     </row>
     <row r="25">
@@ -1540,40 +1565,43 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.1339662447257384</v>
+        <v>0.07383966244725738</v>
       </c>
       <c r="C25" t="n">
-        <v>0.4883966244725738</v>
+        <v>0.3027426160337553</v>
       </c>
       <c r="D25" t="n">
-        <v>0.9978902953586498</v>
+        <v>0.7953586497890295</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9989451476793249</v>
+        <v>0.8976793248945147</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9978902953586498</v>
+        <v>0.9430379746835443</v>
       </c>
       <c r="G25" t="n">
-        <v>1</v>
+        <v>0.9831223628691983</v>
       </c>
       <c r="H25" t="n">
-        <v>0.00949367088607595</v>
+        <v>0.008438818565400843</v>
       </c>
       <c r="I25" t="n">
-        <v>0.9968354430379747</v>
+        <v>0.8132911392405063</v>
       </c>
       <c r="J25" t="n">
-        <v>0.9978902953586498</v>
+        <v>0.9525316455696202</v>
       </c>
       <c r="K25" t="n">
-        <v>28.62173819541931</v>
+        <v>7.86195707321167</v>
       </c>
       <c r="L25" t="n">
-        <v>15.43091702461243</v>
+        <v>2.36637282371521</v>
       </c>
       <c r="M25" t="n">
-        <v>10.789635181427</v>
+        <v>5.149766683578491</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.2680931091308594</v>
       </c>
     </row>
     <row r="26">
@@ -1583,40 +1611,43 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.380564263322884</v>
+        <v>0.3420062695924765</v>
       </c>
       <c r="C26" t="n">
-        <v>0.8771159874608151</v>
+        <v>0.7890282131661442</v>
       </c>
       <c r="D26" t="n">
+        <v>0.9570532915360501</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.9821316614420063</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.9937304075235109</v>
+      </c>
+      <c r="G26" t="n">
         <v>0.9993730407523511</v>
       </c>
-      <c r="E26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.9993730407523511</v>
-      </c>
-      <c r="G26" t="n">
-        <v>1</v>
-      </c>
       <c r="H26" t="n">
-        <v>0.2526645768025078</v>
+        <v>0.2996865203761755</v>
       </c>
       <c r="I26" t="n">
-        <v>0.9993730407523511</v>
+        <v>0.9557993730407524</v>
       </c>
       <c r="J26" t="n">
-        <v>0.9993730407523511</v>
+        <v>0.9968652037617555</v>
       </c>
       <c r="K26" t="n">
-        <v>97.21185851097107</v>
+        <v>27.17301106452942</v>
       </c>
       <c r="L26" t="n">
-        <v>52.23341488838196</v>
+        <v>7.999562978744507</v>
       </c>
       <c r="M26" t="n">
-        <v>36.27751731872559</v>
+        <v>18.00459218025208</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.8971009254455566</v>
       </c>
     </row>
     <row r="27">
@@ -1626,40 +1657,43 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.6066274102297656</v>
+        <v>0.5904629950352154</v>
       </c>
       <c r="C27" t="n">
-        <v>0.9778316591617596</v>
+        <v>0.888696455374668</v>
       </c>
       <c r="D27" t="n">
-        <v>0.9954970557672325</v>
+        <v>0.8430897125043297</v>
       </c>
       <c r="E27" t="n">
-        <v>0.9973444175037525</v>
+        <v>0.9241427086941462</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9966516568525574</v>
+        <v>0.9406535042142939</v>
       </c>
       <c r="G27" t="n">
-        <v>0.9983835584805449</v>
+        <v>0.9787553400300196</v>
       </c>
       <c r="H27" t="n">
-        <v>0.6256783281376285</v>
+        <v>0.5921948966632029</v>
       </c>
       <c r="I27" t="n">
-        <v>0.9957279759842974</v>
+        <v>0.8367394065350422</v>
       </c>
       <c r="J27" t="n">
-        <v>0.9964207366354925</v>
+        <v>0.9475811107262441</v>
       </c>
       <c r="K27" t="n">
-        <v>268.0123617649078</v>
+        <v>73.68007922172546</v>
       </c>
       <c r="L27" t="n">
-        <v>143.4030222892761</v>
+        <v>21.79175710678101</v>
       </c>
       <c r="M27" t="n">
-        <v>98.51647114753723</v>
+        <v>48.74095964431763</v>
+      </c>
+      <c r="N27" t="n">
+        <v>2.432616949081421</v>
       </c>
     </row>
     <row r="28">
@@ -1669,7 +1703,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.4893617021276596</v>
+        <v>0.5319148936170213</v>
       </c>
       <c r="C28" t="n">
         <v>0.9042553191489362</v>
@@ -1678,31 +1712,34 @@
         <v>0.8829787234042553</v>
       </c>
       <c r="E28" t="n">
-        <v>0.9574468085106383</v>
+        <v>0.925531914893617</v>
       </c>
       <c r="F28" t="n">
-        <v>1</v>
+        <v>0.8936170212765957</v>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>0.9361702127659575</v>
       </c>
       <c r="H28" t="n">
-        <v>0.4787234042553192</v>
+        <v>0.4574468085106383</v>
       </c>
       <c r="I28" t="n">
-        <v>0.9042553191489362</v>
+        <v>0.8085106382978723</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>0.8404255319148937</v>
       </c>
       <c r="K28" t="n">
-        <v>2.763039112091064</v>
+        <v>0.8297345638275146</v>
       </c>
       <c r="L28" t="n">
-        <v>1.56317138671875</v>
+        <v>0.2447314262390137</v>
       </c>
       <c r="M28" t="n">
-        <v>1.071576356887817</v>
+        <v>0.5505924224853516</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.02618408203125</v>
       </c>
     </row>
     <row r="29">
@@ -1712,40 +1749,43 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.4794520547945205</v>
+        <v>0.4383561643835616</v>
       </c>
       <c r="C29" t="n">
+        <v>0.821917808219178</v>
+      </c>
+      <c r="D29" t="n">
         <v>0.9178082191780822</v>
       </c>
-      <c r="D29" t="n">
-        <v>1</v>
-      </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>0.9863013698630136</v>
       </c>
       <c r="F29" t="n">
-        <v>1</v>
+        <v>0.9178082191780822</v>
       </c>
       <c r="G29" t="n">
-        <v>1</v>
+        <v>0.9863013698630136</v>
       </c>
       <c r="H29" t="n">
-        <v>0.4520547945205479</v>
+        <v>0.3561643835616438</v>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0.8356164383561644</v>
       </c>
       <c r="J29" t="n">
-        <v>1</v>
+        <v>0.8356164383561644</v>
       </c>
       <c r="K29" t="n">
-        <v>2.289584159851074</v>
+        <v>0.628875732421875</v>
       </c>
       <c r="L29" t="n">
-        <v>1.242538452148438</v>
+        <v>0.185558557510376</v>
       </c>
       <c r="M29" t="n">
-        <v>0.8293333053588867</v>
+        <v>0.4171571731567383</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.02001333236694336</v>
       </c>
     </row>
     <row r="30">
@@ -1755,40 +1795,43 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.6068294239668103</v>
+        <v>0.5096537418222435</v>
       </c>
       <c r="C30" t="n">
-        <v>0.9122387107068773</v>
+        <v>0.7922450933460986</v>
       </c>
       <c r="D30" t="n">
-        <v>0.7924046593266315</v>
+        <v>0.578905377373544</v>
       </c>
       <c r="E30" t="n">
-        <v>0.9475027924046593</v>
+        <v>0.8093186532631244</v>
       </c>
       <c r="F30" t="n">
-        <v>0.7930429232487634</v>
+        <v>0.7265039093665231</v>
       </c>
       <c r="G30" t="n">
-        <v>0.9479814903462582</v>
+        <v>0.8871868517632041</v>
       </c>
       <c r="H30" t="n">
-        <v>0.6081059518110739</v>
+        <v>0.4766235838519228</v>
       </c>
       <c r="I30" t="n">
-        <v>0.800702090314345</v>
+        <v>0.5583213658847933</v>
       </c>
       <c r="J30" t="n">
-        <v>0.8019786181586086</v>
+        <v>0.7229934577947982</v>
       </c>
       <c r="K30" t="n">
-        <v>186.1311571598053</v>
+        <v>52.75604343414307</v>
       </c>
       <c r="L30" t="n">
-        <v>103.0148816108704</v>
+        <v>15.95581531524658</v>
       </c>
       <c r="M30" t="n">
-        <v>71.23478245735168</v>
+        <v>34.80156421661377</v>
+      </c>
+      <c r="N30" t="n">
+        <v>1.482405662536621</v>
       </c>
     </row>
     <row r="31">
@@ -1798,40 +1841,43 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.1737179487179487</v>
+        <v>0.1166666666666667</v>
       </c>
       <c r="C31" t="n">
-        <v>0.5032051282051282</v>
+        <v>0.332051282051282</v>
       </c>
       <c r="D31" t="n">
-        <v>0.8051282051282052</v>
+        <v>0.6076923076923076</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9423076923076923</v>
+        <v>0.808974358974359</v>
       </c>
       <c r="F31" t="n">
-        <v>0.8057692307692308</v>
+        <v>0.791025641025641</v>
       </c>
       <c r="G31" t="n">
-        <v>0.9423076923076923</v>
+        <v>0.9121794871794872</v>
       </c>
       <c r="H31" t="n">
-        <v>0.1102564102564103</v>
+        <v>0.09166666666666666</v>
       </c>
       <c r="I31" t="n">
-        <v>0.8025641025641026</v>
+        <v>0.5967948717948718</v>
       </c>
       <c r="J31" t="n">
-        <v>0.8032051282051282</v>
+        <v>0.8012820512820513</v>
       </c>
       <c r="K31" t="n">
-        <v>45.35229969024658</v>
+        <v>13.15928769111633</v>
       </c>
       <c r="L31" t="n">
-        <v>24.87047171592712</v>
+        <v>3.980528831481934</v>
       </c>
       <c r="M31" t="n">
-        <v>17.68385148048401</v>
+        <v>8.663687944412231</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.3813872337341309</v>
       </c>
     </row>
     <row r="32">
@@ -1841,40 +1887,43 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.8633093525179856</v>
+        <v>0.1007194244604317</v>
       </c>
       <c r="C32" t="n">
-        <v>0.9280575539568345</v>
+        <v>0.2302158273381295</v>
       </c>
       <c r="D32" t="n">
-        <v>0.9496402877697842</v>
+        <v>0.1870503597122302</v>
       </c>
       <c r="E32" t="n">
-        <v>0.9928057553956835</v>
+        <v>0.4172661870503597</v>
       </c>
       <c r="F32" t="n">
-        <v>0.9496402877697842</v>
+        <v>0.1870503597122302</v>
       </c>
       <c r="G32" t="n">
-        <v>0.9928057553956835</v>
+        <v>0.4172661870503597</v>
       </c>
       <c r="H32" t="n">
-        <v>0.8848920863309353</v>
+        <v>0.02877697841726619</v>
       </c>
       <c r="I32" t="n">
-        <v>0.9784172661870504</v>
+        <v>0.1366906474820144</v>
       </c>
       <c r="J32" t="n">
-        <v>0.9784172661870504</v>
+        <v>0.1366906474820144</v>
       </c>
       <c r="K32" t="n">
-        <v>3.809413194656372</v>
+        <v>1.170423984527588</v>
       </c>
       <c r="L32" t="n">
-        <v>2.192337989807129</v>
+        <v>0.3546891212463379</v>
       </c>
       <c r="M32" t="n">
-        <v>1.574325561523438</v>
+        <v>0.764415979385376</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.03955841064453125</v>
       </c>
     </row>
     <row r="33">
@@ -1884,40 +1933,43 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.7560975609756098</v>
+        <v>0.2926829268292683</v>
       </c>
       <c r="C33" t="n">
-        <v>0.926829268292683</v>
+        <v>0.5609756097560976</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>0.8048780487804879</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>0.975609756097561</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>0.8048780487804879</v>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>0.975609756097561</v>
       </c>
       <c r="H33" t="n">
-        <v>0.7073170731707317</v>
+        <v>0.0975609756097561</v>
       </c>
       <c r="I33" t="n">
-        <v>1</v>
+        <v>0.8536585365853658</v>
       </c>
       <c r="J33" t="n">
-        <v>1</v>
+        <v>0.8536585365853658</v>
       </c>
       <c r="K33" t="n">
-        <v>1.186701774597168</v>
+        <v>0.3524250984191895</v>
       </c>
       <c r="L33" t="n">
-        <v>0.7016875743865967</v>
+        <v>0.1097812652587891</v>
       </c>
       <c r="M33" t="n">
-        <v>0.4727389812469482</v>
+        <v>0.2271828651428223</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.01170682907104492</v>
       </c>
     </row>
     <row r="34">
@@ -1927,19 +1979,19 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="C34" t="n">
-        <v>0.2307692307692308</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="D34" t="n">
-        <v>0.9230769230769231</v>
+        <v>1</v>
       </c>
       <c r="E34" t="n">
         <v>1</v>
       </c>
       <c r="F34" t="n">
-        <v>0.9230769230769231</v>
+        <v>1</v>
       </c>
       <c r="G34" t="n">
         <v>1</v>
@@ -1954,13 +2006,16 @@
         <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>0.3872308731079102</v>
+        <v>0.1220991611480713</v>
       </c>
       <c r="L34" t="n">
-        <v>0.2247931957244873</v>
+        <v>0.04009604454040527</v>
       </c>
       <c r="M34" t="n">
-        <v>0.1587927341461182</v>
+        <v>0.07694864273071289</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.003592252731323242</v>
       </c>
     </row>
     <row r="35">
@@ -1970,25 +2025,25 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.4673913043478261</v>
+        <v>0.2826086956521739</v>
       </c>
       <c r="C35" t="n">
-        <v>0.8804347826086957</v>
+        <v>0.6847826086956522</v>
       </c>
       <c r="D35" t="n">
-        <v>0.9456521739130435</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="E35" t="n">
         <v>0.9891304347826086</v>
       </c>
       <c r="F35" t="n">
-        <v>0.9456521739130435</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="G35" t="n">
         <v>0.9891304347826086</v>
       </c>
       <c r="H35" t="n">
-        <v>0.6739130434782609</v>
+        <v>0.09782608695652174</v>
       </c>
       <c r="I35" t="n">
         <v>0.9782608695652174</v>
@@ -1997,13 +2052,16 @@
         <v>0.9782608695652174</v>
       </c>
       <c r="K35" t="n">
-        <v>2.646263599395752</v>
+        <v>0.8183948993682861</v>
       </c>
       <c r="L35" t="n">
-        <v>1.564339160919189</v>
+        <v>0.2329273223876953</v>
       </c>
       <c r="M35" t="n">
-        <v>1.054015398025513</v>
+        <v>0.5514507293701172</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.02610397338867188</v>
       </c>
     </row>
     <row r="36">
@@ -2013,40 +2071,43 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.7647058823529411</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="C36" t="n">
-        <v>0.8235294117647058</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="D36" t="n">
-        <v>0.8235294117647058</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="E36" t="n">
-        <v>0.9411764705882353</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="F36" t="n">
-        <v>0.8235294117647058</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="G36" t="n">
-        <v>0.9411764705882353</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="H36" t="n">
-        <v>0.8235294117647058</v>
+        <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>0.8823529411764706</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="J36" t="n">
-        <v>0.8823529411764706</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="K36" t="n">
-        <v>0.5085687637329102</v>
+        <v>0.1531550884246826</v>
       </c>
       <c r="L36" t="n">
-        <v>0.2929584980010986</v>
+        <v>0.04338693618774414</v>
       </c>
       <c r="M36" t="n">
-        <v>0.2053799629211426</v>
+        <v>0.1034064292907715</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0.004845142364501953</v>
       </c>
     </row>
     <row r="37">
@@ -2062,34 +2123,37 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F37" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G37" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J37" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K37" t="n">
-        <v>0.06941008567810059</v>
+        <v>0.01979923248291016</v>
       </c>
       <c r="L37" t="n">
-        <v>0.04247236251831055</v>
+        <v>0.006103277206420898</v>
       </c>
       <c r="M37" t="n">
-        <v>0.02573752403259277</v>
+        <v>0.01291990280151367</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0.0004212856292724609</v>
       </c>
     </row>
     <row r="38">
@@ -2102,37 +2166,40 @@
         <v>0.25</v>
       </c>
       <c r="C38" t="n">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="F38" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="G38" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
       </c>
       <c r="I38" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="J38" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="K38" t="n">
-        <v>0.226104736328125</v>
+        <v>0.07445955276489258</v>
       </c>
       <c r="L38" t="n">
-        <v>0.1322546005249023</v>
+        <v>0.02163338661193848</v>
       </c>
       <c r="M38" t="n">
-        <v>0.09104800224304199</v>
+        <v>0.04992461204528809</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0.002068281173706055</v>
       </c>
     </row>
     <row r="39">
@@ -2145,37 +2212,40 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F39" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="G39" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="J39" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="K39" t="n">
-        <v>0.2997796535491943</v>
+        <v>0.09391236305236816</v>
       </c>
       <c r="L39" t="n">
-        <v>0.1750028133392334</v>
+        <v>0.0273280143737793</v>
       </c>
       <c r="M39" t="n">
-        <v>0.1213409900665283</v>
+        <v>0.0627753734588623</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0.00265192985534668</v>
       </c>
     </row>
     <row r="40">
@@ -2185,40 +2255,43 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C40" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="E40" t="n">
         <v>1</v>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="G40" t="n">
         <v>1</v>
       </c>
       <c r="H40" t="n">
-        <v>0.2083333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="I40" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="J40" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="K40" t="n">
-        <v>0.6666851043701172</v>
+        <v>0.2126584053039551</v>
       </c>
       <c r="L40" t="n">
-        <v>0.3856956958770752</v>
+        <v>0.06540846824645996</v>
       </c>
       <c r="M40" t="n">
-        <v>0.2723293304443359</v>
+        <v>0.1385033130645752</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0.006552457809448242</v>
       </c>
     </row>
     <row r="41">
@@ -2228,40 +2301,43 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>0.375</v>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="F41" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G41" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="H41" t="n">
-        <v>0.625</v>
+        <v>0.125</v>
       </c>
       <c r="I41" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="J41" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="K41" t="n">
-        <v>0.2473764419555664</v>
+        <v>0.07458853721618652</v>
       </c>
       <c r="L41" t="n">
-        <v>0.1441755294799805</v>
+        <v>0.02277350425720215</v>
       </c>
       <c r="M41" t="n">
-        <v>0.1011500358581543</v>
+        <v>0.04876089096069336</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0.002144575119018555</v>
       </c>
     </row>
     <row r="42">
@@ -2271,40 +2347,43 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.4444444444444444</v>
+        <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="E42" t="n">
         <v>1</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="G42" t="n">
         <v>1</v>
       </c>
       <c r="H42" t="n">
-        <v>0.4444444444444444</v>
+        <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="J42" t="n">
-        <v>1</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="K42" t="n">
-        <v>0.2657809257507324</v>
+        <v>0.09277868270874023</v>
       </c>
       <c r="L42" t="n">
-        <v>0.1551949977874756</v>
+        <v>0.03280878067016602</v>
       </c>
       <c r="M42" t="n">
-        <v>0.1086115837097168</v>
+        <v>0.0567467212677002</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0.002110719680786133</v>
       </c>
     </row>
     <row r="43">
@@ -2317,16 +2396,16 @@
         <v>0.125</v>
       </c>
       <c r="C43" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D43" t="n">
         <v>0.875</v>
       </c>
-      <c r="D43" t="n">
-        <v>1</v>
-      </c>
       <c r="E43" t="n">
         <v>1</v>
       </c>
       <c r="F43" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="G43" t="n">
         <v>1</v>
@@ -2335,19 +2414,22 @@
         <v>0</v>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="J43" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="K43" t="n">
-        <v>0.223466157913208</v>
+        <v>0.07252955436706543</v>
       </c>
       <c r="L43" t="n">
-        <v>0.1306190490722656</v>
+        <v>0.02132511138916016</v>
       </c>
       <c r="M43" t="n">
-        <v>0.09120631217956543</v>
+        <v>0.04823660850524902</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0.002132892608642578</v>
       </c>
     </row>
     <row r="44">
@@ -2357,25 +2439,25 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="C44" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D44" t="n">
         <v>0.875</v>
       </c>
-      <c r="D44" t="n">
-        <v>1</v>
-      </c>
       <c r="E44" t="n">
         <v>1</v>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="G44" t="n">
         <v>1</v>
       </c>
       <c r="H44" t="n">
-        <v>0.375</v>
+        <v>0</v>
       </c>
       <c r="I44" t="n">
         <v>1</v>
@@ -2384,13 +2466,16 @@
         <v>1</v>
       </c>
       <c r="K44" t="n">
-        <v>0.2238552570343018</v>
+        <v>0.07022380828857422</v>
       </c>
       <c r="L44" t="n">
-        <v>0.130882740020752</v>
+        <v>0.02129268646240234</v>
       </c>
       <c r="M44" t="n">
-        <v>0.0912327766418457</v>
+        <v>0.04588007926940918</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0.00214385986328125</v>
       </c>
     </row>
     <row r="45">
@@ -2400,10 +2485,10 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="C45" t="n">
-        <v>1</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="D45" t="n">
         <v>1</v>
@@ -2418,7 +2503,7 @@
         <v>1</v>
       </c>
       <c r="H45" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="I45" t="n">
         <v>1</v>
@@ -2427,13 +2512,16 @@
         <v>1</v>
       </c>
       <c r="K45" t="n">
-        <v>0.4996709823608398</v>
+        <v>0.1616535186767578</v>
       </c>
       <c r="L45" t="n">
-        <v>0.2908492088317871</v>
+        <v>0.04631757736206055</v>
       </c>
       <c r="M45" t="n">
-        <v>0.2047641277313232</v>
+        <v>0.1085379123687744</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0.005127906799316406</v>
       </c>
     </row>
     <row r="46">
@@ -2443,40 +2531,43 @@
         </is>
       </c>
       <c r="B46" t="n">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C46" t="n">
         <v>0.7777777777777778</v>
       </c>
-      <c r="C46" t="n">
-        <v>1</v>
-      </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>0.9722222222222222</v>
       </c>
       <c r="F46" t="n">
-        <v>1</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="G46" t="n">
-        <v>1</v>
+        <v>0.9722222222222222</v>
       </c>
       <c r="H46" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.25</v>
       </c>
       <c r="I46" t="n">
-        <v>1</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="J46" t="n">
-        <v>1</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="K46" t="n">
-        <v>0.9983735084533691</v>
+        <v>0.3228611946105957</v>
       </c>
       <c r="L46" t="n">
-        <v>0.5826699733734131</v>
+        <v>0.09098362922668457</v>
       </c>
       <c r="M46" t="n">
-        <v>0.4086811542510986</v>
+        <v>0.2179162502288818</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0.01087403297424316</v>
       </c>
     </row>
     <row r="47">
@@ -2486,40 +2577,43 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="C47" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E47" t="n">
         <v>0.95</v>
       </c>
-      <c r="D47" t="n">
-        <v>1</v>
-      </c>
-      <c r="E47" t="n">
-        <v>1</v>
-      </c>
       <c r="F47" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G47" t="n">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="H47" t="n">
-        <v>0.6</v>
+        <v>0.35</v>
       </c>
       <c r="I47" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="J47" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K47" t="n">
-        <v>0.5666391849517822</v>
+        <v>0.1804802417755127</v>
       </c>
       <c r="L47" t="n">
-        <v>0.3307681083679199</v>
+        <v>0.05040287971496582</v>
       </c>
       <c r="M47" t="n">
-        <v>0.2321112155914307</v>
+        <v>0.1221737861633301</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0.006029367446899414</v>
       </c>
     </row>
     <row r="48">
@@ -2529,40 +2623,43 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>1</v>
+        <v>0.5652173913043478</v>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>0.7391304347826086</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>0.5652173913043478</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>0.7391304347826086</v>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>0.5652173913043478</v>
       </c>
       <c r="G48" t="n">
-        <v>1</v>
+        <v>0.7391304347826086</v>
       </c>
       <c r="H48" t="n">
-        <v>1</v>
+        <v>0.4347826086956522</v>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>0.4347826086956522</v>
       </c>
       <c r="J48" t="n">
-        <v>1</v>
+        <v>0.4347826086956522</v>
       </c>
       <c r="K48" t="n">
-        <v>0.7328534126281738</v>
+        <v>0.2082829475402832</v>
       </c>
       <c r="L48" t="n">
-        <v>0.4258112907409668</v>
+        <v>0.05897784233093262</v>
       </c>
       <c r="M48" t="n">
-        <v>0.2878537178039551</v>
+        <v>0.1403043270111084</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0.00696563720703125</v>
       </c>
     </row>
     <row r="49">
@@ -2572,40 +2669,43 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="F49" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G49" t="n">
-        <v>1</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="H49" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="I49" t="n">
-        <v>1</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="J49" t="n">
-        <v>1</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="K49" t="n">
-        <v>0.4881629943847656</v>
+        <v>0.1207537651062012</v>
       </c>
       <c r="L49" t="n">
-        <v>0.262315034866333</v>
+        <v>0.03715062141418457</v>
       </c>
       <c r="M49" t="n">
-        <v>0.1595113277435303</v>
+        <v>0.07846164703369141</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0.003828287124633789</v>
       </c>
     </row>
     <row r="50">
@@ -2615,40 +2715,43 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.8780487804878049</v>
+        <v>0.7073170731707317</v>
       </c>
       <c r="C50" t="n">
-        <v>0.926829268292683</v>
+        <v>0.8536585365853658</v>
       </c>
       <c r="D50" t="n">
-        <v>0.8902439024390244</v>
+        <v>0.7195121951219512</v>
       </c>
       <c r="E50" t="n">
-        <v>0.926829268292683</v>
+        <v>0.8536585365853658</v>
       </c>
       <c r="F50" t="n">
-        <v>0.8902439024390244</v>
+        <v>0.7195121951219512</v>
       </c>
       <c r="G50" t="n">
-        <v>0.926829268292683</v>
+        <v>0.8536585365853658</v>
       </c>
       <c r="H50" t="n">
-        <v>0.8780487804878049</v>
+        <v>0.5609756097560976</v>
       </c>
       <c r="I50" t="n">
-        <v>0.8902439024390244</v>
+        <v>0.5853658536585366</v>
       </c>
       <c r="J50" t="n">
-        <v>0.8902439024390244</v>
+        <v>0.5853658536585366</v>
       </c>
       <c r="K50" t="n">
-        <v>2.70607590675354</v>
+        <v>0.7017848491668701</v>
       </c>
       <c r="L50" t="n">
-        <v>1.492794990539551</v>
+        <v>0.2100841999053955</v>
       </c>
       <c r="M50" t="n">
-        <v>0.9355185031890869</v>
+        <v>0.4616115093231201</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0.02280330657958984</v>
       </c>
     </row>
     <row r="51">
@@ -2658,40 +2761,43 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.25</v>
+        <v>0.0625</v>
       </c>
       <c r="C51" t="n">
-        <v>0.5</v>
+        <v>0.15625</v>
       </c>
       <c r="D51" t="n">
-        <v>0.46875</v>
+        <v>0.15625</v>
       </c>
       <c r="E51" t="n">
-        <v>0.75</v>
+        <v>0.4375</v>
       </c>
       <c r="F51" t="n">
-        <v>0.46875</v>
+        <v>0.15625</v>
       </c>
       <c r="G51" t="n">
-        <v>0.75</v>
+        <v>0.4375</v>
       </c>
       <c r="H51" t="n">
-        <v>0.09375</v>
+        <v>0</v>
       </c>
       <c r="I51" t="n">
-        <v>0.5625</v>
+        <v>0.15625</v>
       </c>
       <c r="J51" t="n">
-        <v>0.5625</v>
+        <v>0.15625</v>
       </c>
       <c r="K51" t="n">
-        <v>0.9410498142242432</v>
+        <v>0.289320707321167</v>
       </c>
       <c r="L51" t="n">
-        <v>0.5478689670562744</v>
+        <v>0.08306145668029785</v>
       </c>
       <c r="M51" t="n">
-        <v>0.36515212059021</v>
+        <v>0.1945140361785889</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0.008887052536010742</v>
       </c>
     </row>
     <row r="52">
@@ -2701,40 +2807,43 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.5700483091787439</v>
+        <v>0.1400966183574879</v>
       </c>
       <c r="C52" t="n">
-        <v>0.9082125603864735</v>
+        <v>0.4009661835748792</v>
       </c>
       <c r="D52" t="n">
-        <v>0.7198067632850241</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E52" t="n">
-        <v>0.9758454106280193</v>
+        <v>0.8647342995169082</v>
       </c>
       <c r="F52" t="n">
-        <v>0.7198067632850241</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G52" t="n">
-        <v>0.9758454106280193</v>
+        <v>0.8647342995169082</v>
       </c>
       <c r="H52" t="n">
-        <v>0.6183574879227053</v>
+        <v>0.07246376811594203</v>
       </c>
       <c r="I52" t="n">
-        <v>0.7826086956521739</v>
+        <v>0.6570048309178744</v>
       </c>
       <c r="J52" t="n">
-        <v>0.7826086956521739</v>
+        <v>0.6570048309178744</v>
       </c>
       <c r="K52" t="n">
-        <v>5.915372610092163</v>
+        <v>1.788079023361206</v>
       </c>
       <c r="L52" t="n">
-        <v>3.491508960723877</v>
+        <v>0.5329771041870117</v>
       </c>
       <c r="M52" t="n">
-        <v>2.356030702590942</v>
+        <v>1.17818021774292</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0.05813264846801758</v>
       </c>
     </row>
     <row r="53">
@@ -2744,40 +2853,43 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.6526315789473685</v>
+        <v>0.2631578947368421</v>
       </c>
       <c r="C53" t="n">
-        <v>0.8631578947368421</v>
+        <v>0.6631578947368421</v>
       </c>
       <c r="D53" t="n">
+        <v>0.9157894736842105</v>
+      </c>
+      <c r="E53" t="n">
         <v>0.9894736842105263</v>
       </c>
-      <c r="E53" t="n">
-        <v>1</v>
-      </c>
       <c r="F53" t="n">
+        <v>0.9157894736842105</v>
+      </c>
+      <c r="G53" t="n">
         <v>0.9894736842105263</v>
       </c>
-      <c r="G53" t="n">
-        <v>1</v>
-      </c>
       <c r="H53" t="n">
-        <v>0.6</v>
+        <v>0.1157894736842105</v>
       </c>
       <c r="I53" t="n">
-        <v>0.9894736842105263</v>
+        <v>0.9157894736842105</v>
       </c>
       <c r="J53" t="n">
-        <v>0.9894736842105263</v>
+        <v>0.9157894736842105</v>
       </c>
       <c r="K53" t="n">
-        <v>2.642330169677734</v>
+        <v>0.845555305480957</v>
       </c>
       <c r="L53" t="n">
-        <v>1.52579402923584</v>
+        <v>0.2445487976074219</v>
       </c>
       <c r="M53" t="n">
-        <v>1.086335897445679</v>
+        <v>0.5663993358612061</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0.02663159370422363</v>
       </c>
     </row>
     <row r="54">
@@ -2787,40 +2899,43 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.8773006134969326</v>
+        <v>0.656441717791411</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9631901840490797</v>
+        <v>0.901840490797546</v>
       </c>
       <c r="D54" t="n">
-        <v>1</v>
+        <v>0.9570552147239264</v>
       </c>
       <c r="E54" t="n">
         <v>1</v>
       </c>
       <c r="F54" t="n">
-        <v>1</v>
+        <v>0.9570552147239264</v>
       </c>
       <c r="G54" t="n">
         <v>1</v>
       </c>
       <c r="H54" t="n">
-        <v>0.8650306748466258</v>
+        <v>0.5828220858895705</v>
       </c>
       <c r="I54" t="n">
-        <v>1</v>
+        <v>0.9877300613496932</v>
       </c>
       <c r="J54" t="n">
-        <v>1</v>
+        <v>0.9877300613496932</v>
       </c>
       <c r="K54" t="n">
-        <v>4.45801854133606</v>
+        <v>1.407352924346924</v>
       </c>
       <c r="L54" t="n">
-        <v>2.562247753143311</v>
+        <v>0.4197163581848145</v>
       </c>
       <c r="M54" t="n">
-        <v>1.845620632171631</v>
+        <v>0.9265468120574951</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0.04664301872253418</v>
       </c>
     </row>
     <row r="55">
@@ -2830,40 +2945,43 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.2962962962962963</v>
+        <v>0.1481481481481481</v>
       </c>
       <c r="C55" t="n">
-        <v>0.4259259259259259</v>
+        <v>0.2777777777777778</v>
       </c>
       <c r="D55" t="n">
         <v>0.6296296296296297</v>
       </c>
       <c r="E55" t="n">
-        <v>0.7962962962962963</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="F55" t="n">
         <v>0.6296296296296297</v>
       </c>
       <c r="G55" t="n">
-        <v>0.7962962962962963</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="H55" t="n">
-        <v>0.3148148148148148</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="I55" t="n">
-        <v>0.6481481481481481</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J55" t="n">
-        <v>0.6481481481481481</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="K55" t="n">
-        <v>1.483102560043335</v>
+        <v>0.4718685150146484</v>
       </c>
       <c r="L55" t="n">
-        <v>0.8528621196746826</v>
+        <v>0.1427359580993652</v>
       </c>
       <c r="M55" t="n">
-        <v>0.6120510101318359</v>
+        <v>0.3089323043823242</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0.01515531539916992</v>
       </c>
     </row>
     <row r="56">
@@ -2873,40 +2991,43 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="E56" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="G56" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
       </c>
       <c r="I56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K56" t="n">
-        <v>0.09291839599609375</v>
+        <v>0.02917695045471191</v>
       </c>
       <c r="L56" t="n">
-        <v>0.05710434913635254</v>
+        <v>0.009209632873535156</v>
       </c>
       <c r="M56" t="n">
-        <v>0.03462672233581543</v>
+        <v>0.01907110214233398</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0.000484466552734375</v>
       </c>
     </row>
     <row r="57">
@@ -2916,40 +3037,43 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.8125</v>
+        <v>0.4375</v>
       </c>
       <c r="C57" t="n">
-        <v>0.828125</v>
+        <v>0.640625</v>
       </c>
       <c r="D57" t="n">
-        <v>0.921875</v>
+        <v>0.875</v>
       </c>
       <c r="E57" t="n">
-        <v>0.953125</v>
+        <v>0.96875</v>
       </c>
       <c r="F57" t="n">
-        <v>0.921875</v>
+        <v>0.875</v>
       </c>
       <c r="G57" t="n">
-        <v>0.953125</v>
+        <v>0.96875</v>
       </c>
       <c r="H57" t="n">
-        <v>0.78125</v>
+        <v>0.265625</v>
       </c>
       <c r="I57" t="n">
-        <v>0.921875</v>
+        <v>0.859375</v>
       </c>
       <c r="J57" t="n">
-        <v>0.921875</v>
+        <v>0.859375</v>
       </c>
       <c r="K57" t="n">
-        <v>1.837544918060303</v>
+        <v>0.5648818016052246</v>
       </c>
       <c r="L57" t="n">
-        <v>1.086560249328613</v>
+        <v>0.1792061328887939</v>
       </c>
       <c r="M57" t="n">
-        <v>0.7299022674560547</v>
+        <v>0.3621242046356201</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0.01726269721984863</v>
       </c>
     </row>
     <row r="58">
@@ -2959,40 +3083,43 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.336734693877551</v>
+        <v>0.173469387755102</v>
       </c>
       <c r="C58" t="n">
-        <v>0.5204081632653061</v>
+        <v>0.3673469387755102</v>
       </c>
       <c r="D58" t="n">
-        <v>0.7346938775510204</v>
+        <v>0.4693877551020408</v>
       </c>
       <c r="E58" t="n">
-        <v>0.9081632653061225</v>
+        <v>0.6020408163265306</v>
       </c>
       <c r="F58" t="n">
-        <v>0.7346938775510204</v>
+        <v>0.4693877551020408</v>
       </c>
       <c r="G58" t="n">
-        <v>0.9081632653061225</v>
+        <v>0.6020408163265306</v>
       </c>
       <c r="H58" t="n">
-        <v>0.2755102040816326</v>
+        <v>0.1020408163265306</v>
       </c>
       <c r="I58" t="n">
-        <v>0.7346938775510204</v>
+        <v>0.4897959183673469</v>
       </c>
       <c r="J58" t="n">
-        <v>0.7346938775510204</v>
+        <v>0.4897959183673469</v>
       </c>
       <c r="K58" t="n">
-        <v>2.74235987663269</v>
+        <v>0.8640639781951904</v>
       </c>
       <c r="L58" t="n">
-        <v>1.56489634513855</v>
+        <v>0.2569155693054199</v>
       </c>
       <c r="M58" t="n">
-        <v>1.109081506729126</v>
+        <v>0.5711517333984375</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0.02779102325439453</v>
       </c>
     </row>
     <row r="59">
@@ -3002,10 +3129,10 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
         <v>1</v>
@@ -3020,7 +3147,7 @@
         <v>1</v>
       </c>
       <c r="H59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" t="n">
         <v>1</v>
@@ -3029,13 +3156,16 @@
         <v>1</v>
       </c>
       <c r="K59" t="n">
-        <v>0.03400874137878418</v>
+        <v>0.01097679138183594</v>
       </c>
       <c r="L59" t="n">
-        <v>0.02112007141113281</v>
+        <v>0.003551006317138672</v>
       </c>
       <c r="M59" t="n">
-        <v>0.01180481910705566</v>
+        <v>0.007058143615722656</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0.0001442432403564453</v>
       </c>
     </row>
     <row r="60">
@@ -3063,22 +3193,25 @@
         <v>1</v>
       </c>
       <c r="H60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60" t="n">
-        <v>0.03417730331420898</v>
+        <v>0.01134896278381348</v>
       </c>
       <c r="L60" t="n">
-        <v>0.02135396003723145</v>
+        <v>0.003577709197998047</v>
       </c>
       <c r="M60" t="n">
-        <v>0.0118110179901123</v>
+        <v>0.007389068603515625</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0.0001330375671386719</v>
       </c>
     </row>
     <row r="61">
@@ -3106,22 +3239,25 @@
         <v>1</v>
       </c>
       <c r="H61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" t="n">
         <v>1</v>
       </c>
       <c r="K61" t="n">
-        <v>0.03704333305358887</v>
+        <v>0.01050972938537598</v>
       </c>
       <c r="L61" t="n">
-        <v>0.02298879623413086</v>
+        <v>0.003652811050415039</v>
       </c>
       <c r="M61" t="n">
-        <v>0.01310563087463379</v>
+        <v>0.006551265716552734</v>
+      </c>
+      <c r="N61" t="n">
+        <v>8.654594421386719e-05</v>
       </c>
     </row>
     <row r="62">
@@ -3158,13 +3294,16 @@
         <v>1</v>
       </c>
       <c r="K62" t="n">
-        <v>0.03418779373168945</v>
+        <v>0.01180171966552734</v>
       </c>
       <c r="L62" t="n">
-        <v>0.02139401435852051</v>
+        <v>0.003808736801147461</v>
       </c>
       <c r="M62" t="n">
-        <v>0.01184797286987305</v>
+        <v>0.007628679275512695</v>
+      </c>
+      <c r="N62" t="n">
+        <v>0.0001187324523925781</v>
       </c>
     </row>
     <row r="63">
@@ -3174,16 +3313,16 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C63" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D63" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E63" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>1</v>
@@ -3192,22 +3331,25 @@
         <v>1</v>
       </c>
       <c r="H63" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I63" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J63" t="n">
         <v>1</v>
       </c>
       <c r="K63" t="n">
-        <v>0.06812214851379395</v>
+        <v>0.02061605453491211</v>
       </c>
       <c r="L63" t="n">
-        <v>0.04103183746337891</v>
+        <v>0.006247758865356445</v>
       </c>
       <c r="M63" t="n">
-        <v>0.0256493091583252</v>
+        <v>0.01361489295959473</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0.0004189014434814453</v>
       </c>
     </row>
     <row r="64">
@@ -3217,26 +3359,26 @@
         </is>
       </c>
       <c r="B64" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1</v>
+      </c>
+      <c r="F64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G64" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" t="n">
         <v>0</v>
       </c>
-      <c r="C64" t="n">
-        <v>1</v>
-      </c>
-      <c r="D64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E64" t="n">
-        <v>1</v>
-      </c>
-      <c r="F64" t="n">
-        <v>1</v>
-      </c>
-      <c r="G64" t="n">
-        <v>1</v>
-      </c>
-      <c r="H64" t="n">
-        <v>1</v>
-      </c>
       <c r="I64" t="n">
         <v>1</v>
       </c>
@@ -3244,13 +3386,16 @@
         <v>1</v>
       </c>
       <c r="K64" t="n">
-        <v>0.03718876838684082</v>
+        <v>0.01137280464172363</v>
       </c>
       <c r="L64" t="n">
-        <v>0.02304959297180176</v>
+        <v>0.003748416900634766</v>
       </c>
       <c r="M64" t="n">
-        <v>0.0131840705871582</v>
+        <v>0.007210016250610352</v>
+      </c>
+      <c r="N64" t="n">
+        <v>0.0001175403594970703</v>
       </c>
     </row>
     <row r="65">
@@ -3260,7 +3405,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65" t="n">
         <v>1</v>
@@ -3278,22 +3423,25 @@
         <v>1</v>
       </c>
       <c r="H65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K65" t="n">
-        <v>0.03708744049072266</v>
+        <v>0.01147031784057617</v>
       </c>
       <c r="L65" t="n">
-        <v>0.0230867862701416</v>
+        <v>0.00360870361328125</v>
       </c>
       <c r="M65" t="n">
-        <v>0.01303362846374512</v>
+        <v>0.007472753524780273</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0.0001342296600341797</v>
       </c>
     </row>
     <row r="66">
@@ -3330,13 +3478,16 @@
         <v>1</v>
       </c>
       <c r="K66" t="n">
-        <v>0.03394985198974609</v>
+        <v>0.01157164573669434</v>
       </c>
       <c r="L66" t="n">
-        <v>0.02119755744934082</v>
+        <v>0.003736019134521484</v>
       </c>
       <c r="M66" t="n">
-        <v>0.01180291175842285</v>
+        <v>0.007446527481079102</v>
+      </c>
+      <c r="N66" t="n">
+        <v>0.0001342296600341797</v>
       </c>
     </row>
     <row r="67">
@@ -3346,40 +3497,43 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.647887323943662</v>
+        <v>0.4859154929577465</v>
       </c>
       <c r="C67" t="n">
-        <v>0.9471830985915493</v>
+        <v>0.7535211267605634</v>
       </c>
       <c r="D67" t="n">
-        <v>0.9647887323943662</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="E67" t="n">
-        <v>0.9753521126760564</v>
+        <v>0.8838028169014085</v>
       </c>
       <c r="F67" t="n">
-        <v>0.9647887323943662</v>
+        <v>0.6901408450704225</v>
       </c>
       <c r="G67" t="n">
-        <v>0.9753521126760564</v>
+        <v>0.8838028169014085</v>
       </c>
       <c r="H67" t="n">
-        <v>0.6866197183098591</v>
+        <v>0.3873239436619718</v>
       </c>
       <c r="I67" t="n">
-        <v>0.9612676056338029</v>
+        <v>0.6091549295774648</v>
       </c>
       <c r="J67" t="n">
-        <v>0.9612676056338029</v>
+        <v>0.6091549295774648</v>
       </c>
       <c r="K67" t="n">
-        <v>7.782314300537109</v>
+        <v>2.375238418579102</v>
       </c>
       <c r="L67" t="n">
-        <v>4.462785720825195</v>
+        <v>0.7218186855316162</v>
       </c>
       <c r="M67" t="n">
-        <v>3.217789173126221</v>
+        <v>1.549396276473999</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0.08039522171020508</v>
       </c>
     </row>
     <row r="68">
@@ -3389,40 +3543,43 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.5324074074074074</v>
+        <v>0.462962962962963</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9305555555555556</v>
+        <v>0.8101851851851852</v>
       </c>
       <c r="D68" t="n">
-        <v>0.9861111111111112</v>
+        <v>0.6990740740740741</v>
       </c>
       <c r="E68" t="n">
-        <v>0.9861111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="F68" t="n">
-        <v>0.9861111111111112</v>
+        <v>0.6990740740740741</v>
       </c>
       <c r="G68" t="n">
-        <v>0.9861111111111112</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="H68" t="n">
-        <v>0.4675925925925926</v>
+        <v>0.412037037037037</v>
       </c>
       <c r="I68" t="n">
-        <v>0.9861111111111112</v>
+        <v>0.7037037037037037</v>
       </c>
       <c r="J68" t="n">
-        <v>0.9861111111111112</v>
+        <v>0.7037037037037037</v>
       </c>
       <c r="K68" t="n">
-        <v>5.917368412017822</v>
+        <v>1.87025260925293</v>
       </c>
       <c r="L68" t="n">
-        <v>3.390887498855591</v>
+        <v>0.5581932067871094</v>
       </c>
       <c r="M68" t="n">
-        <v>2.444336414337158</v>
+        <v>1.232209444046021</v>
+      </c>
+      <c r="N68" t="n">
+        <v>0.06137919425964355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>